<commit_message>
Add sheets to roo functionality
</commit_message>
<xml_diff>
--- a/spec/fixtures/facebook_comments2.xlsx
+++ b/spec/fixtures/facebook_comments2.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t>Date of Message</t>
   </si>
@@ -241,16 +242,104 @@
   <si>
     <t>Mary Till</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Comment Type
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1. Reply to Original Message
+2. Reply to another user
+3. Tag Another user in comment
+4. Share / Retweet with comment
+5. Link to Article/Blog/Other Website</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>In the US, about 20% of all deaths are caused by a #smoking-related disease every year. http://bit.ly/2pxp6Lt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">;) </t>
+  </si>
+  <si>
+    <t>10sdab</t>
+  </si>
+  <si>
+    <t>Probably a bot/spam - Q. Le @ 21 Jun 2017</t>
+  </si>
+  <si>
+    <t>Smoking #cigarettes can claim more than 10 years of your life. Don’t let #cigs cut your life short. http://bit.ly/2oqdFR7</t>
+  </si>
+  <si>
+    <t>This is nice :)</t>
+  </si>
+  <si>
+    <t>cigarfanaticsworld</t>
+  </si>
+  <si>
+    <t>Using #tobacco products can lead to addiction and expose people to toxic, cancer-causing chemicals. http://bit.ly/2qchj3o</t>
+  </si>
+  <si>
+    <t>Awesome shots loving your gallery! #MrBrog</t>
+  </si>
+  <si>
+    <t>mrbrog</t>
+  </si>
+  <si>
+    <t>Over 100 million non-smokers in this country are exposed to toxic secondhand smoke. http://bit.ly/2qrdtTT #smoking</t>
+  </si>
+  <si>
+    <t>Wow! I love this photo :D</t>
+  </si>
+  <si>
+    <t>elfbreadshop</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,8 +395,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -317,6 +411,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB4C6E7"/>
+        <bgColor rgb="FFB4C6E7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor rgb="FFB4C6E7"/>
       </patternFill>
     </fill>
@@ -348,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -399,6 +499,36 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,7 +811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -845,4 +975,179 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="168" x14ac:dyDescent="0.25">
+      <c r="A2" s="23">
+        <v>42846</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="24">
+        <v>42846</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="11">
+        <v>1</v>
+      </c>
+      <c r="G2" s="26">
+        <v>1</v>
+      </c>
+      <c r="H2" s="26">
+        <v>10</v>
+      </c>
+      <c r="I2" s="26">
+        <v>12</v>
+      </c>
+      <c r="J2" s="27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="168" x14ac:dyDescent="0.25">
+      <c r="A3" s="24">
+        <v>42850</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="24">
+        <v>42850</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="11">
+        <v>1</v>
+      </c>
+      <c r="G3" s="26">
+        <v>1</v>
+      </c>
+      <c r="H3" s="26">
+        <v>1</v>
+      </c>
+      <c r="I3" s="26">
+        <v>12</v>
+      </c>
+      <c r="J3" s="27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="192" x14ac:dyDescent="0.25">
+      <c r="A4" s="23">
+        <v>42855</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="24">
+        <v>42855</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="11">
+        <v>1</v>
+      </c>
+      <c r="G4" s="26">
+        <v>1</v>
+      </c>
+      <c r="H4" s="26">
+        <v>1</v>
+      </c>
+      <c r="I4" s="26">
+        <v>12</v>
+      </c>
+      <c r="J4" s="27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+      <c r="A5" s="24">
+        <v>42861</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="24">
+        <v>42861</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="11">
+        <v>1</v>
+      </c>
+      <c r="G5" s="26">
+        <v>1</v>
+      </c>
+      <c r="H5" s="26">
+        <v>1</v>
+      </c>
+      <c r="I5" s="26">
+        <v>12</v>
+      </c>
+      <c r="J5" s="27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Acts as codeable (#415)
* merge

* Fix merge conflicts
</commit_message>
<xml_diff>
--- a/spec/fixtures/facebook_comments2.xlsx
+++ b/spec/fixtures/facebook_comments2.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t>Date of Message</t>
   </si>
@@ -241,16 +242,104 @@
   <si>
     <t>Mary Till</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Comment Type
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1. Reply to Original Message
+2. Reply to another user
+3. Tag Another user in comment
+4. Share / Retweet with comment
+5. Link to Article/Blog/Other Website</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>In the US, about 20% of all deaths are caused by a #smoking-related disease every year. http://bit.ly/2pxp6Lt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">;) </t>
+  </si>
+  <si>
+    <t>10sdab</t>
+  </si>
+  <si>
+    <t>Probably a bot/spam - Q. Le @ 21 Jun 2017</t>
+  </si>
+  <si>
+    <t>Smoking #cigarettes can claim more than 10 years of your life. Don’t let #cigs cut your life short. http://bit.ly/2oqdFR7</t>
+  </si>
+  <si>
+    <t>This is nice :)</t>
+  </si>
+  <si>
+    <t>cigarfanaticsworld</t>
+  </si>
+  <si>
+    <t>Using #tobacco products can lead to addiction and expose people to toxic, cancer-causing chemicals. http://bit.ly/2qchj3o</t>
+  </si>
+  <si>
+    <t>Awesome shots loving your gallery! #MrBrog</t>
+  </si>
+  <si>
+    <t>mrbrog</t>
+  </si>
+  <si>
+    <t>Over 100 million non-smokers in this country are exposed to toxic secondhand smoke. http://bit.ly/2qrdtTT #smoking</t>
+  </si>
+  <si>
+    <t>Wow! I love this photo :D</t>
+  </si>
+  <si>
+    <t>elfbreadshop</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,8 +395,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -317,6 +411,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB4C6E7"/>
+        <bgColor rgb="FFB4C6E7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor rgb="FFB4C6E7"/>
       </patternFill>
     </fill>
@@ -348,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -399,6 +499,36 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,7 +811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -845,4 +975,179 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="168" x14ac:dyDescent="0.25">
+      <c r="A2" s="23">
+        <v>42846</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="24">
+        <v>42846</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="11">
+        <v>1</v>
+      </c>
+      <c r="G2" s="26">
+        <v>1</v>
+      </c>
+      <c r="H2" s="26">
+        <v>10</v>
+      </c>
+      <c r="I2" s="26">
+        <v>12</v>
+      </c>
+      <c r="J2" s="27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="168" x14ac:dyDescent="0.25">
+      <c r="A3" s="24">
+        <v>42850</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="24">
+        <v>42850</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="11">
+        <v>1</v>
+      </c>
+      <c r="G3" s="26">
+        <v>1</v>
+      </c>
+      <c r="H3" s="26">
+        <v>1</v>
+      </c>
+      <c r="I3" s="26">
+        <v>12</v>
+      </c>
+      <c r="J3" s="27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="192" x14ac:dyDescent="0.25">
+      <c r="A4" s="23">
+        <v>42855</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="24">
+        <v>42855</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="11">
+        <v>1</v>
+      </c>
+      <c r="G4" s="26">
+        <v>1</v>
+      </c>
+      <c r="H4" s="26">
+        <v>1</v>
+      </c>
+      <c r="I4" s="26">
+        <v>12</v>
+      </c>
+      <c r="J4" s="27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+      <c r="A5" s="24">
+        <v>42861</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="24">
+        <v>42861</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="11">
+        <v>1</v>
+      </c>
+      <c r="G5" s="26">
+        <v>1</v>
+      </c>
+      <c r="H5" s="26">
+        <v>1</v>
+      </c>
+      <c r="I5" s="26">
+        <v>12</v>
+      </c>
+      <c r="J5" s="27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>